<commit_message>
Nye testdata Debitor og Økonomi
</commit_message>
<xml_diff>
--- a/SF1590_C ØiR - Afsend udbetalingsanmodninger til ØiR (Udbetalinger)/Documentation/Arkiv/G68 testdata hjælpeark.xlsx
+++ b/SF1590_C ØiR - Afsend udbetalingsanmodninger til ØiR (Udbetalinger)/Documentation/Arkiv/G68 testdata hjælpeark.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srv-a2-dc01\folders$\jho\Documents\GitHub\SOATest\SF1590_C ØiR - Afsend udbetalingsanmodninger til ØiR (Udbetalinger)\Documentation\Arkiv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="7680"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="11652" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="104">
   <si>
     <t>Felt nr.</t>
   </si>
@@ -126,9 +126,6 @@
     <t>UDBETALINGSDATO</t>
   </si>
   <si>
-    <t>00000000</t>
-  </si>
-  <si>
     <t>FILLER</t>
   </si>
   <si>
@@ -243,21 +240,12 @@
     <t>20160701</t>
   </si>
   <si>
-    <t>0117</t>
-  </si>
-  <si>
     <t>033</t>
   </si>
   <si>
-    <t>0751</t>
-  </si>
-  <si>
     <t>0000834633</t>
   </si>
   <si>
-    <t xml:space="preserve">G68-TST1-RUN01    </t>
-  </si>
-  <si>
     <t>00000101604888</t>
   </si>
   <si>
@@ -267,9 +255,6 @@
     <t xml:space="preserve">          </t>
   </si>
   <si>
-    <t xml:space="preserve">                   </t>
-  </si>
-  <si>
     <t xml:space="preserve">                    </t>
   </si>
   <si>
@@ -297,9 +282,6 @@
     <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                  </t>
   </si>
   <si>
-    <t>000000006801</t>
-  </si>
-  <si>
     <t>Transaktionsdato</t>
   </si>
   <si>
@@ -328,12 +310,33 @@
   </si>
   <si>
     <t>G68 testdata hjælpeark</t>
+  </si>
+  <si>
+    <t>0450</t>
+  </si>
+  <si>
+    <t>0252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G68-TST10-RUN03   </t>
+  </si>
+  <si>
+    <t>000000005804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">71011100000000005  </t>
+  </si>
+  <si>
+    <t>0084957631</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -376,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -411,6 +414,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,9 +441,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -475,7 +481,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -510,6 +516,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -545,9 +568,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -723,18 +763,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.125" style="6"/>
-    <col min="3" max="6" width="20.125" style="12"/>
-    <col min="7" max="16384" width="20.125" style="6"/>
+    <col min="1" max="2" width="20.08984375" style="6"/>
+    <col min="3" max="6" width="20.08984375" style="12"/>
+    <col min="7" max="16384" width="20.08984375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -749,13 +791,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -771,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="14">
         <f>LEN(C4)</f>
@@ -824,8 +866,8 @@
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>77</v>
+      <c r="C6" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="14">
         <f t="shared" si="0"/>
@@ -851,8 +893,8 @@
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>76</v>
+      <c r="C7" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="D7" s="14">
         <f t="shared" si="0"/>
@@ -906,7 +948,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="14">
         <f t="shared" si="0"/>
@@ -933,7 +975,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D10" s="14">
         <f t="shared" si="0"/>
@@ -960,7 +1002,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="14">
         <f t="shared" si="0"/>
@@ -987,7 +1029,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="0"/>
@@ -1014,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D13" s="14">
         <f t="shared" si="0"/>
@@ -1095,7 +1137,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D16" s="14">
         <f t="shared" si="0"/>
@@ -1122,7 +1164,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="D17" s="14">
         <f t="shared" si="0"/>
@@ -1146,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>3</v>
@@ -1170,10 +1212,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>5</v>
@@ -1200,10 +1242,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="D20" s="14">
         <f t="shared" si="0"/>
@@ -1227,10 +1269,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D21" s="14">
         <f t="shared" si="0"/>
@@ -1251,13 +1293,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D22" s="14">
         <f t="shared" si="0"/>
@@ -1278,13 +1320,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D23" s="14">
         <f t="shared" si="0"/>
@@ -1305,13 +1347,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="C24" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D24" s="14">
         <f t="shared" si="0"/>
@@ -1332,13 +1374,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D25" s="14">
         <f t="shared" si="0"/>
@@ -1359,13 +1401,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="C26" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D26" s="14">
         <f t="shared" si="0"/>
@@ -1386,13 +1428,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="C27" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D27" s="14">
         <f t="shared" si="0"/>
@@ -1413,13 +1455,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D28" s="14">
         <f t="shared" si="0"/>
@@ -1441,10 +1483,10 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D29" s="14">
         <f t="shared" si="0"/>
@@ -1465,13 +1507,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>58</v>
       </c>
       <c r="D30" s="14">
         <f t="shared" si="0"/>
@@ -1492,13 +1534,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="D31" s="14">
         <f t="shared" si="0"/>
@@ -1519,13 +1561,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="C32" s="10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D32" s="14">
         <f t="shared" si="0"/>
@@ -1549,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D33" s="14">
         <f t="shared" si="0"/>
@@ -1573,13 +1615,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="C34" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D34" s="14">
         <f t="shared" si="0"/>
@@ -1600,13 +1642,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="C35" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D35" s="14">
         <f t="shared" si="0"/>
@@ -1627,13 +1669,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="D36" s="14">
         <f t="shared" si="0"/>
@@ -1655,10 +1697,10 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D37" s="14">
         <f t="shared" si="0"/>
@@ -1680,10 +1722,10 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D38" s="14">
         <f t="shared" si="0"/>
@@ -1705,10 +1747,10 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D39" s="14">
         <f t="shared" si="0"/>
@@ -1741,22 +1783,22 @@
         <v>0</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C41" s="15">
-        <v>42658</v>
+        <v>42737</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C42" s="14">
         <v>1</v>
@@ -1764,25 +1806,25 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B43" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C43" s="12" t="str">
-        <f>CONCATENATE("Z300 ",$C$7,"6      ",_xlfn.DAYS($C$41,DATE(2016,1,1))+1,"0   G68")</f>
-        <v>Z300 07516      2890   G68</v>
+        <f>CONCATENATE("Z300 ",$C$7,"6      ",_xlfn.DAYS($C$41,DATE(2017,1,1))+1,"0   G68")</f>
+        <v>Z300 04506      20   G68</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C44" s="12" t="str">
         <f>CONCATENATE(C4,C5,C6,C7,C8,C9,C10,C11,C12,C13,C14,C15,C16,C17,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C39)</f>
-        <v xml:space="preserve">0030000834633075101          0117033G68-TST1-RUN01    000000006801+020000010160488800000000 00                                                                                                                                                                0000               52001234560                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                        20160701G68KBIT     DKK                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         </v>
+        <v xml:space="preserve">0630000834633045001          0252033G68-TST10-RUN03   000000005804+0200000101604888         0071011100000000005                          0084957631                                                                                                           0000               52001234560                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                        20160701G68KBIT     DKK                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         </v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C45" s="12" t="str">
         <f>CONCATENATE("SLUTD",IF(LEN($C$42)=1,"0000",IF(LEN($C$42)=2,"000",IF(LEN($C$42)=3,"00",IF(LEN($C$42)=4,"0",IF(LEN($C$42)=5,"","00000"))))),$C$42)</f>
@@ -1802,6 +1844,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008E0B7D38E4258844897A19598B2E0E1C" ma:contentTypeVersion="2" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="1522932ced3d8d0fbbdc0236e42ef527">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3fe48988bd14f1f5287e128ef4d8b91b" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1947,31 +2013,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F44DDD4D-E43A-48D0-ADB3-8219FF5B0680}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB867D05-8470-422F-A974-0D414FFB0255}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01400007-0071-476B-9690-E42A5B457041}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1987,28 +2053,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB867D05-8470-422F-A974-0D414FFB0255}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F44DDD4D-E43A-48D0-ADB3-8219FF5B0680}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>